<commit_message>
feat: work progress, match and select, query doc
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/报价单/Copy of 凌威报价单2.13(1).xlsx
+++ b/报价单/Copy of 凌威报价单2.13(1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1774\Documents\xwechat_files\wxid_mzgv071wte3822_ae76\msg\file\2026-02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\agent-jk\Agent Team version3\报价单\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{275EB683-784E-48D3-B21D-B66CD5CF3692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FCEE35-D884-4806-8F4C-2A2200F65DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>万鼎国际集团                                                         VANTSING INTERNATIONAL GROUP</t>
   </si>
@@ -1063,11 +1063,11 @@
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0_);\(#,##0.0\)"/>
-    <numFmt numFmtId="169" formatCode="0_ "/>
-    <numFmt numFmtId="170" formatCode="0.00_ "/>
-    <numFmt numFmtId="171" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="172" formatCode="[$Rp-421]#,##0;\-[$Rp-421]#,##0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0_);\(#,##0.0\)"/>
+    <numFmt numFmtId="167" formatCode="0_ "/>
+    <numFmt numFmtId="168" formatCode="0.00_ "/>
+    <numFmt numFmtId="169" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="170" formatCode="[$Rp-421]#,##0;\-[$Rp-421]#,##0"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1097,7 +1097,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1233,7 +1233,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1493,7 +1493,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
@@ -1519,7 +1519,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1558,7 +1558,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1570,16 +1570,16 @@
     <xf numFmtId="165" fontId="23" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1600,152 +1600,152 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="22" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="22" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2166,7 +2166,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="56" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
@@ -2195,31 +2195,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" customFormat="1" ht="195" customHeight="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="40" t="e" vm="1">
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="78" t="e" vm="1">
         <f ca="1">_xlfn.DISPIMG("ID_2AB6C2DF03EC4B189D9084FA977CA6E6",1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="42"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="80"/>
     </row>
     <row r="2" spans="1:18" ht="70.05" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -2424,15 +2424,9 @@
       <c r="H7" s="20"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="14">
-        <v>450</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="19"/>
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
@@ -2470,230 +2464,230 @@
       <c r="R8" s="31"/>
     </row>
     <row r="9" spans="1:18" s="3" customFormat="1" ht="64.95" customHeight="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="47"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="83"/>
       <c r="O9" s="26"/>
       <c r="P9" s="26"/>
       <c r="Q9" s="32"/>
       <c r="R9" s="31"/>
     </row>
     <row r="10" spans="1:18" s="3" customFormat="1" ht="64.95" customHeight="1">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="50"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="72"/>
       <c r="O10" s="26"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="33"/>
       <c r="R10" s="32"/>
     </row>
     <row r="11" spans="1:18" s="3" customFormat="1" ht="64.95" customHeight="1">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="26"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="32"/>
     </row>
     <row r="12" spans="1:18" s="3" customFormat="1" ht="60" customHeight="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="55"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="60"/>
       <c r="O12" s="26"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="34"/>
       <c r="R12" s="34"/>
     </row>
     <row r="13" spans="1:18" s="3" customFormat="1" ht="60" customHeight="1">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="55"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="60"/>
     </row>
     <row r="14" spans="1:18" ht="60" customHeight="1">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="62"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="63"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="65"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="67"/>
     </row>
     <row r="15" spans="1:18" ht="60" customHeight="1">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="63"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="65"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="67"/>
     </row>
     <row r="16" spans="1:18" ht="60" customHeight="1">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="64" t="s">
+      <c r="J16" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="64"/>
-      <c r="L16" s="65">
+      <c r="K16" s="45"/>
+      <c r="L16" s="47">
         <v>46066</v>
       </c>
-      <c r="M16" s="65"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="65"/>
-      <c r="R16" s="66"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="48"/>
     </row>
     <row r="17" spans="1:18" ht="70.05" customHeight="1">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="68"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="67" t="s">
+      <c r="J17" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="67"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="73"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="55"/>
     </row>
     <row r="18" spans="1:18" s="4" customFormat="1" ht="22.05" customHeight="1">
-      <c r="A18" s="74" t="s">
+      <c r="A18" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
     </row>
     <row r="19" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A19" s="17" t="s">
@@ -2702,24 +2696,24 @@
       <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
     </row>
     <row r="20" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A20" s="17">
@@ -2728,24 +2722,24 @@
       <c r="B20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
     </row>
     <row r="21" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A21" s="17">
@@ -2754,24 +2748,24 @@
       <c r="B21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="77"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="77"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
     </row>
     <row r="22" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A22" s="17">
@@ -2780,22 +2774,22 @@
       <c r="B22" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="78"/>
-      <c r="O22" s="78"/>
-      <c r="P22" s="78"/>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="78"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
     </row>
     <row r="23" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A23" s="17">
@@ -2804,338 +2798,373 @@
       <c r="B23" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
     </row>
     <row r="24" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A24" s="75">
+      <c r="A24" s="39">
         <v>5</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="78" t="s">
+      <c r="C24" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="78"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
     </row>
     <row r="25" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A25" s="75"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="80"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="80"/>
-      <c r="Q25" s="80"/>
-      <c r="R25" s="80"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
     </row>
     <row r="26" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A26" s="75"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="80" t="s">
+      <c r="C26" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
-      <c r="L26" s="80"/>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80"/>
-      <c r="O26" s="80"/>
-      <c r="P26" s="80"/>
-      <c r="Q26" s="80"/>
-      <c r="R26" s="80"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
     </row>
     <row r="27" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="75"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
-      <c r="I27" s="80"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="80"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="80"/>
-      <c r="N27" s="80"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="80"/>
-      <c r="Q27" s="80"/>
-      <c r="R27" s="80"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
     </row>
     <row r="28" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A28" s="75"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
-      <c r="L28" s="80"/>
-      <c r="M28" s="80"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="80"/>
-      <c r="P28" s="80"/>
-      <c r="Q28" s="80"/>
-      <c r="R28" s="80"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
     </row>
     <row r="29" spans="1:18" s="4" customFormat="1" ht="27" customHeight="1">
-      <c r="A29" s="75"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="81"/>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="81"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
     </row>
     <row r="30" spans="1:18" s="4" customFormat="1" ht="25.05" customHeight="1">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="81"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="81"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
     </row>
     <row r="31" spans="1:18" s="4" customFormat="1" ht="25.05" customHeight="1">
-      <c r="A31" s="81"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="81"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="81"/>
-      <c r="M31" s="81"/>
-      <c r="N31" s="81"/>
-      <c r="O31" s="81"/>
-      <c r="P31" s="81"/>
-      <c r="Q31" s="81"/>
-      <c r="R31" s="81"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
     </row>
     <row r="32" spans="1:18" s="5" customFormat="1" ht="40.950000000000003" customHeight="1">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="82" t="s">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="82"/>
-      <c r="J32" s="82"/>
-      <c r="K32" s="82"/>
-      <c r="L32" s="82"/>
-      <c r="M32" s="82"/>
-      <c r="N32" s="82"/>
-      <c r="O32" s="82"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="82"/>
-      <c r="R32" s="82"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
     </row>
     <row r="33" spans="1:18" s="5" customFormat="1" ht="13.8">
-      <c r="A33" s="83"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83"/>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="83"/>
-      <c r="M33" s="83"/>
-      <c r="N33" s="83"/>
-      <c r="O33" s="83"/>
-      <c r="P33" s="83"/>
-      <c r="Q33" s="83"/>
-      <c r="R33" s="83"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
     </row>
     <row r="34" spans="1:18" s="5" customFormat="1" ht="13.8">
-      <c r="A34" s="83"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="83"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83"/>
-      <c r="J34" s="83"/>
-      <c r="K34" s="83"/>
-      <c r="L34" s="83"/>
-      <c r="M34" s="83"/>
-      <c r="N34" s="83"/>
-      <c r="O34" s="83"/>
-      <c r="P34" s="83"/>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="83"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
     </row>
     <row r="35" spans="1:18" s="5" customFormat="1" ht="13.8">
-      <c r="A35" s="83"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
-      <c r="N35" s="83"/>
-      <c r="O35" s="83"/>
-      <c r="P35" s="83"/>
-      <c r="Q35" s="83"/>
-      <c r="R35" s="83"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
     </row>
     <row r="36" spans="1:18" s="5" customFormat="1" ht="13.8">
-      <c r="A36" s="83"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="83"/>
-      <c r="N36" s="83"/>
-      <c r="O36" s="83"/>
-      <c r="P36" s="83"/>
-      <c r="Q36" s="83"/>
-      <c r="R36" s="83"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
     </row>
     <row r="37" spans="1:18" s="5" customFormat="1" ht="46.05" customHeight="1">
-      <c r="A37" s="83"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="83"/>
-      <c r="N37" s="83"/>
-      <c r="O37" s="83"/>
-      <c r="P37" s="83"/>
-      <c r="Q37" s="83"/>
-      <c r="R37" s="83"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:R32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="43">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:R13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:R14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:R15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:R16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:R17"/>
+    <mergeCell ref="A18:R18"/>
+    <mergeCell ref="C19:R19"/>
+    <mergeCell ref="C20:R20"/>
+    <mergeCell ref="C21:R21"/>
+    <mergeCell ref="C22:R22"/>
+    <mergeCell ref="C23:R23"/>
+    <mergeCell ref="C24:R24"/>
+    <mergeCell ref="C25:R25"/>
+    <mergeCell ref="C26:R26"/>
+    <mergeCell ref="C27:R27"/>
     <mergeCell ref="A33:G37"/>
     <mergeCell ref="A30:R31"/>
     <mergeCell ref="H33:R37"/>
@@ -3144,41 +3173,6 @@
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="H32:R32"/>
     <mergeCell ref="A24:A29"/>
-    <mergeCell ref="C23:R23"/>
-    <mergeCell ref="C24:R24"/>
-    <mergeCell ref="C25:R25"/>
-    <mergeCell ref="C26:R26"/>
-    <mergeCell ref="C27:R27"/>
-    <mergeCell ref="A18:R18"/>
-    <mergeCell ref="C19:R19"/>
-    <mergeCell ref="C20:R20"/>
-    <mergeCell ref="C21:R21"/>
-    <mergeCell ref="C22:R22"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:R16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:R17"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:R13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:R14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:R15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:N9"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A8">
     <cfRule type="duplicateValues" dxfId="1" priority="129"/>

</xml_diff>